<commit_message>
edit Cases and Check files
</commit_message>
<xml_diff>
--- a/Check.xlsx
+++ b/Check.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikit\Downloads\fmh_android_15_03_24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4CB3CA5-7A55-48DF-8742-FCACFBD04852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75183236-F0BB-4BF6-8B31-B07322C5B88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="-120" windowWidth="27645" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6600" yWindow="2400" windowWidth="19500" windowHeight="11220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="64">
   <si>
     <t>Приоритет</t>
   </si>
@@ -208,6 +208,15 @@
   </si>
   <si>
     <t>Вкладка "About" в главном меню</t>
+  </si>
+  <si>
+    <t>Ручное тестирование</t>
+  </si>
+  <si>
+    <t>Пройден</t>
+  </si>
+  <si>
+    <t>Не пройден</t>
   </si>
 </sst>
 </file>
@@ -246,7 +255,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -255,15 +264,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -548,11 +548,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -572,111 +607,113 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -684,11 +721,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -696,14 +736,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -988,7 +1029,7 @@
   <dimension ref="A1:M226"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,7 +1040,7 @@
     <col min="4" max="4" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>5</v>
       </c>
@@ -1011,6 +1052,9 @@
       </c>
       <c r="D1" s="19" t="s">
         <v>0</v>
+      </c>
+      <c r="E1" s="50" t="s">
+        <v>61</v>
       </c>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -1021,8 +1065,8 @@
       <c r="L1" s="3"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
+    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="41" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="15" t="s">
@@ -1031,11 +1075,13 @@
       <c r="C2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="21"/>
-      <c r="F2" s="3"/>
+      <c r="E2" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" s="6"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -1044,8 +1090,8 @@
       <c r="L2" s="3"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="44"/>
+    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="42"/>
       <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
@@ -1055,7 +1101,9 @@
       <c r="D3" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="21"/>
+      <c r="E3" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -1065,8 +1113,8 @@
       <c r="L3" s="3"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="44"/>
+    <row r="4" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="42"/>
       <c r="B4" s="7" t="s">
         <v>8</v>
       </c>
@@ -1076,7 +1124,9 @@
       <c r="D4" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="21"/>
+      <c r="E4" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -1086,8 +1136,8 @@
       <c r="L4" s="3"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="44"/>
+    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="42"/>
       <c r="B5" s="7" t="s">
         <v>9</v>
       </c>
@@ -1097,7 +1147,9 @@
       <c r="D5" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="21"/>
+      <c r="E5" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -1107,8 +1159,8 @@
       <c r="L5" s="3"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
+    <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="42"/>
       <c r="B6" s="8" t="s">
         <v>10</v>
       </c>
@@ -1118,8 +1170,10 @@
       <c r="D6" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="3"/>
+      <c r="E6" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="6"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -1128,9 +1182,9 @@
       <c r="L6" s="3"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="45"/>
-      <c r="B7" s="41" t="s">
+    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="43"/>
+      <c r="B7" s="39" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -1139,7 +1193,9 @@
       <c r="D7" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="21"/>
+      <c r="E7" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -1150,17 +1206,19 @@
       <c r="M7" s="1"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="46"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="11" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="21"/>
+      <c r="E8" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -1170,8 +1228,8 @@
       <c r="L8" s="3"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="47" t="s">
+    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="45" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="12" t="s">
@@ -1180,10 +1238,12 @@
       <c r="C9" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -1193,8 +1253,8 @@
       <c r="L9" s="3"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="48"/>
+    <row r="10" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="46"/>
       <c r="B10" s="9" t="s">
         <v>20</v>
       </c>
@@ -1204,7 +1264,9 @@
       <c r="D10" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="25"/>
+      <c r="E10" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -1214,8 +1276,8 @@
       <c r="L10" s="3"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="48"/>
+    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="46"/>
       <c r="B11" s="9" t="s">
         <v>21</v>
       </c>
@@ -1225,7 +1287,9 @@
       <c r="D11" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="25"/>
+      <c r="E11" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -1235,8 +1299,8 @@
       <c r="L11" s="3"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="48"/>
+    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="46"/>
       <c r="B12" s="9" t="s">
         <v>22</v>
       </c>
@@ -1246,7 +1310,9 @@
       <c r="D12" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="25"/>
+      <c r="E12" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -1256,9 +1322,9 @@
       <c r="L12" s="3"/>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="49"/>
-      <c r="B13" s="42" t="s">
+    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="47"/>
+      <c r="B13" s="40" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="7" t="s">
@@ -1267,7 +1333,9 @@
       <c r="D13" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="25"/>
+      <c r="E13" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -1278,17 +1346,19 @@
       <c r="M13" s="1"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="49"/>
-      <c r="B14" s="24" t="s">
+      <c r="A14" s="47"/>
+      <c r="B14" s="23" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="27" t="s">
+      <c r="D14" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="25"/>
+      <c r="E14" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -1299,19 +1369,21 @@
       <c r="M14" s="1"/>
     </row>
     <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="32" t="s">
+      <c r="D15" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="25"/>
+      <c r="E15" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -1321,20 +1393,22 @@
       <c r="L15" s="3"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="50" t="s">
+    <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="28" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="3"/>
+      <c r="E16" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -1344,18 +1418,20 @@
       <c r="L16" s="3"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="48"/>
+    <row r="17" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="46"/>
       <c r="B17" s="10" t="s">
         <v>27</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="33" t="s">
+      <c r="D17" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="6"/>
+      <c r="E17" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -1365,18 +1441,20 @@
       <c r="L17" s="3"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="48"/>
+    <row r="18" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="46"/>
       <c r="B18" s="10" t="s">
         <v>28</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="33" t="s">
+      <c r="D18" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E18" s="3"/>
+      <c r="E18" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -1386,18 +1464,20 @@
       <c r="L18" s="3"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="48"/>
+    <row r="19" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="46"/>
       <c r="B19" s="10" t="s">
         <v>29</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="33" t="s">
+      <c r="D19" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="3"/>
+      <c r="E19" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -1407,18 +1487,20 @@
       <c r="L19" s="3"/>
       <c r="M19" s="1"/>
     </row>
-    <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="48"/>
+    <row r="20" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="46"/>
       <c r="B20" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="33" t="s">
+      <c r="D20" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E20" s="3"/>
+      <c r="E20" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -1428,18 +1510,20 @@
       <c r="L20" s="3"/>
       <c r="M20" s="1"/>
     </row>
-    <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="48"/>
+    <row r="21" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="46"/>
       <c r="B21" s="10" t="s">
         <v>31</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="33" t="s">
+      <c r="D21" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="3"/>
+      <c r="E21" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
@@ -1449,18 +1533,20 @@
       <c r="L21" s="3"/>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="48"/>
+    <row r="22" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="46"/>
       <c r="B22" s="10" t="s">
         <v>32</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D22" s="33" t="s">
+      <c r="D22" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="3"/>
+      <c r="E22" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -1470,18 +1556,20 @@
       <c r="L22" s="3"/>
       <c r="M22" s="1"/>
     </row>
-    <row r="23" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="48"/>
+    <row r="23" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="46"/>
       <c r="B23" s="10" t="s">
         <v>33</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="33" t="s">
+      <c r="D23" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="3"/>
+      <c r="E23" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
@@ -1491,18 +1579,20 @@
       <c r="L23" s="3"/>
       <c r="M23" s="1"/>
     </row>
-    <row r="24" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="48"/>
+    <row r="24" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="46"/>
       <c r="B24" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="33" t="s">
+      <c r="D24" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E24" s="3"/>
+      <c r="E24" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -1512,18 +1602,20 @@
       <c r="L24" s="3"/>
       <c r="M24" s="1"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="48"/>
+    <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="46"/>
       <c r="B25" s="10" t="s">
         <v>35</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D25" s="33" t="s">
+      <c r="D25" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="3"/>
+      <c r="E25" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -1533,18 +1625,20 @@
       <c r="L25" s="3"/>
       <c r="M25" s="1"/>
     </row>
-    <row r="26" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="48"/>
+    <row r="26" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="46"/>
       <c r="B26" s="10" t="s">
         <v>36</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="33" t="s">
+      <c r="D26" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E26" s="3"/>
+      <c r="E26" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
@@ -1554,18 +1648,20 @@
       <c r="L26" s="3"/>
       <c r="M26" s="1"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="48"/>
+    <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="46"/>
       <c r="B27" s="10" t="s">
         <v>37</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="33" t="s">
+      <c r="D27" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E27" s="3"/>
+      <c r="E27" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
@@ -1575,18 +1671,20 @@
       <c r="L27" s="3"/>
       <c r="M27" s="1"/>
     </row>
-    <row r="28" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="48"/>
+    <row r="28" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="46"/>
       <c r="B28" s="10" t="s">
         <v>38</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D28" s="33" t="s">
+      <c r="D28" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E28" s="3"/>
+      <c r="E28" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
@@ -1596,18 +1694,20 @@
       <c r="L28" s="3"/>
       <c r="M28" s="1"/>
     </row>
-    <row r="29" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="48"/>
+    <row r="29" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="46"/>
       <c r="B29" s="10" t="s">
         <v>39</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D29" s="33" t="s">
+      <c r="D29" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E29" s="3"/>
+      <c r="E29" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
@@ -1617,18 +1717,20 @@
       <c r="L29" s="3"/>
       <c r="M29" s="1"/>
     </row>
-    <row r="30" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="48"/>
+    <row r="30" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="46"/>
       <c r="B30" s="10" t="s">
         <v>40</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D30" s="33" t="s">
+      <c r="D30" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E30" s="3"/>
+      <c r="E30" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
@@ -1638,18 +1740,20 @@
       <c r="L30" s="3"/>
       <c r="M30" s="1"/>
     </row>
-    <row r="31" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="48"/>
+    <row r="31" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="46"/>
       <c r="B31" s="10" t="s">
         <v>41</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D31" s="33" t="s">
+      <c r="D31" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E31" s="3"/>
+      <c r="E31" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
@@ -1659,18 +1763,20 @@
       <c r="L31" s="3"/>
       <c r="M31" s="1"/>
     </row>
-    <row r="32" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="48"/>
+    <row r="32" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="46"/>
       <c r="B32" s="10" t="s">
         <v>42</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D32" s="33" t="s">
+      <c r="D32" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E32" s="3"/>
+      <c r="E32" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
@@ -1680,18 +1786,20 @@
       <c r="L32" s="3"/>
       <c r="M32" s="1"/>
     </row>
-    <row r="33" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="48"/>
+    <row r="33" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="46"/>
       <c r="B33" s="10" t="s">
         <v>43</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D33" s="33" t="s">
+      <c r="D33" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E33" s="3"/>
+      <c r="E33" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
@@ -1701,18 +1809,20 @@
       <c r="L33" s="3"/>
       <c r="M33" s="1"/>
     </row>
-    <row r="34" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="48"/>
+    <row r="34" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="46"/>
       <c r="B34" s="10" t="s">
         <v>44</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D34" s="33" t="s">
+      <c r="D34" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E34" s="3"/>
+      <c r="E34" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
@@ -1722,18 +1832,20 @@
       <c r="L34" s="3"/>
       <c r="M34" s="1"/>
     </row>
-    <row r="35" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="48"/>
+    <row r="35" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="46"/>
       <c r="B35" s="10" t="s">
         <v>45</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D35" s="33" t="s">
+      <c r="D35" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E35" s="3"/>
+      <c r="E35" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
@@ -1743,18 +1855,20 @@
       <c r="L35" s="3"/>
       <c r="M35" s="1"/>
     </row>
-    <row r="36" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="48"/>
+    <row r="36" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="46"/>
       <c r="B36" s="10" t="s">
         <v>46</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D36" s="33" t="s">
+      <c r="D36" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E36" s="3"/>
+      <c r="E36" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
@@ -1764,18 +1878,20 @@
       <c r="L36" s="3"/>
       <c r="M36" s="1"/>
     </row>
-    <row r="37" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="48"/>
+    <row r="37" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="46"/>
       <c r="B37" s="10" t="s">
         <v>47</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D37" s="33" t="s">
+      <c r="D37" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E37" s="3"/>
+      <c r="E37" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
@@ -1785,18 +1901,20 @@
       <c r="L37" s="3"/>
       <c r="M37" s="1"/>
     </row>
-    <row r="38" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="48"/>
+    <row r="38" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="46"/>
       <c r="B38" s="10" t="s">
         <v>48</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="33" t="s">
+      <c r="D38" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E38" s="3"/>
+      <c r="E38" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
@@ -1806,18 +1924,20 @@
       <c r="L38" s="3"/>
       <c r="M38" s="1"/>
     </row>
-    <row r="39" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="48"/>
+    <row r="39" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="46"/>
       <c r="B39" s="10" t="s">
         <v>49</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D39" s="33" t="s">
+      <c r="D39" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E39" s="3"/>
+      <c r="E39" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
@@ -1827,18 +1947,20 @@
       <c r="L39" s="3"/>
       <c r="M39" s="1"/>
     </row>
-    <row r="40" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="48"/>
+    <row r="40" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="46"/>
       <c r="B40" s="10" t="s">
         <v>50</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D40" s="33" t="s">
+      <c r="D40" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E40" s="3"/>
+      <c r="E40" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
@@ -1848,18 +1970,20 @@
       <c r="L40" s="3"/>
       <c r="M40" s="1"/>
     </row>
-    <row r="41" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="48"/>
+    <row r="41" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="46"/>
       <c r="B41" s="10" t="s">
         <v>51</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D41" s="33" t="s">
+      <c r="D41" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E41" s="3"/>
+      <c r="E41" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
@@ -1869,18 +1993,20 @@
       <c r="L41" s="3"/>
       <c r="M41" s="1"/>
     </row>
-    <row r="42" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="48"/>
+    <row r="42" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="46"/>
       <c r="B42" s="10" t="s">
         <v>52</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D42" s="33" t="s">
+      <c r="D42" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E42" s="3"/>
+      <c r="E42" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
@@ -1890,18 +2016,20 @@
       <c r="L42" s="3"/>
       <c r="M42" s="1"/>
     </row>
-    <row r="43" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="48"/>
+    <row r="43" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="46"/>
       <c r="B43" s="10" t="s">
         <v>53</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D43" s="33" t="s">
+      <c r="D43" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E43" s="3"/>
+      <c r="E43" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
@@ -1911,18 +2039,20 @@
       <c r="L43" s="3"/>
       <c r="M43" s="1"/>
     </row>
-    <row r="44" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="48"/>
+    <row r="44" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="46"/>
       <c r="B44" s="10" t="s">
         <v>54</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D44" s="33" t="s">
+      <c r="D44" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E44" s="3"/>
+      <c r="E44" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
@@ -1932,18 +2062,20 @@
       <c r="L44" s="3"/>
       <c r="M44" s="1"/>
     </row>
-    <row r="45" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="48"/>
+    <row r="45" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="46"/>
       <c r="B45" s="10" t="s">
         <v>56</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D45" s="33" t="s">
+      <c r="D45" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E45" s="3"/>
+      <c r="E45" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
@@ -1954,17 +2086,19 @@
       <c r="M45" s="1"/>
     </row>
     <row r="46" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="51"/>
-      <c r="B46" s="34" t="s">
+      <c r="A46" s="49"/>
+      <c r="B46" s="32" t="s">
         <v>55</v>
       </c>
       <c r="C46" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D46" s="37" t="s">
+      <c r="D46" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="E46" s="3"/>
+      <c r="E46" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
@@ -1975,19 +2109,21 @@
       <c r="M46" s="1"/>
     </row>
     <row r="47" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="38" t="s">
+      <c r="A47" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B47" s="39" t="s">
+      <c r="B47" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="C47" s="31" t="s">
+      <c r="C47" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="D47" s="40" t="s">
+      <c r="D47" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="E47" s="25"/>
+      <c r="E47" s="52" t="s">
+        <v>62</v>
+      </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
@@ -1997,20 +2133,22 @@
       <c r="L47" s="3"/>
       <c r="M47" s="1"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="47" t="s">
+    <row r="48" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="B48" s="35" t="s">
+      <c r="B48" s="33" t="s">
         <v>58</v>
       </c>
       <c r="C48" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D48" s="36" t="s">
+      <c r="D48" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="E48" s="25"/>
+      <c r="E48" s="53" t="s">
+        <v>63</v>
+      </c>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
@@ -2020,18 +2158,20 @@
       <c r="L48" s="3"/>
       <c r="M48" s="1"/>
     </row>
-    <row r="49" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="51"/>
-      <c r="B49" s="34" t="s">
+    <row r="49" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="49"/>
+      <c r="B49" s="32" t="s">
         <v>59</v>
       </c>
       <c r="C49" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D49" s="27" t="s">
+      <c r="D49" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E49" s="25"/>
+      <c r="E49" s="53" t="s">
+        <v>63</v>
+      </c>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
@@ -2046,7 +2186,7 @@
       <c r="B50" s="4"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
+      <c r="E50" s="51"/>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>

</xml_diff>